<commit_message>
feat: Added Database Connection and Funcationality to Every Form in The Admin Panel
</commit_message>
<xml_diff>
--- a/Project Proposal/Simple Gantt chart1.xlsx
+++ b/Project Proposal/Simple Gantt chart1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssaro\Documents\My Docs\LA Grandee BCA\4th Semester\Project\Project Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssaro\Documents\My Docs\LA Grandee BCA\4th Semester\PU-BCA-4th-Semester-Project\Project Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4813080-1451-460E-B797-3ECFAAB40C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C781DBC4-227D-4451-A8A6-140CBDAFD15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>PROGRESS</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Retrospect Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              </t>
   </si>
 </sst>
 </file>
@@ -911,15 +914,46 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="21" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -935,45 +969,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1601,387 +1604,389 @@
       <c r="D1" s="17"/>
       <c r="E1" s="18"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
       <c r="O1" s="20"/>
-      <c r="P1" s="71">
+      <c r="P1" s="82">
         <f ca="1">TODAY()-5</f>
-        <v>45409</v>
-      </c>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
+        <v>45444</v>
+      </c>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
       <c r="O2" s="20"/>
-      <c r="P2" s="69">
+      <c r="P2" s="80">
         <v>1</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
     </row>
     <row r="3" spans="1:63" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D3" s="24"/>
-      <c r="H3" s="66">
+      <c r="H3" s="87">
         <f ca="1">H4</f>
-        <v>45404</v>
-      </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64">
+        <v>45439</v>
+      </c>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85">
         <f ca="1">O4</f>
-        <v>45411</v>
-      </c>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64">
+        <v>45446</v>
+      </c>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85">
         <f ca="1">V4</f>
-        <v>45418</v>
-      </c>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64">
+        <v>45453</v>
+      </c>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85">
         <f ca="1">AC4</f>
-        <v>45425</v>
-      </c>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64">
+        <v>45460</v>
+      </c>
+      <c r="AD3" s="85"/>
+      <c r="AE3" s="85"/>
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="85"/>
+      <c r="AJ3" s="85">
         <f ca="1">AJ4</f>
-        <v>45432</v>
-      </c>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64">
+        <v>45467</v>
+      </c>
+      <c r="AK3" s="85"/>
+      <c r="AL3" s="85"/>
+      <c r="AM3" s="85"/>
+      <c r="AN3" s="85"/>
+      <c r="AO3" s="85"/>
+      <c r="AP3" s="85"/>
+      <c r="AQ3" s="85">
         <f ca="1">AQ4</f>
-        <v>45439</v>
-      </c>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="64"/>
-      <c r="AX3" s="64">
+        <v>45474</v>
+      </c>
+      <c r="AR3" s="85"/>
+      <c r="AS3" s="85"/>
+      <c r="AT3" s="85"/>
+      <c r="AU3" s="85"/>
+      <c r="AV3" s="85"/>
+      <c r="AW3" s="85"/>
+      <c r="AX3" s="85">
         <f ca="1">AX4</f>
-        <v>45446</v>
-      </c>
-      <c r="AY3" s="64"/>
-      <c r="AZ3" s="64"/>
-      <c r="BA3" s="64"/>
-      <c r="BB3" s="64"/>
-      <c r="BC3" s="64"/>
-      <c r="BD3" s="64"/>
-      <c r="BE3" s="64">
+        <v>45481</v>
+      </c>
+      <c r="AY3" s="85"/>
+      <c r="AZ3" s="85"/>
+      <c r="BA3" s="85"/>
+      <c r="BB3" s="85"/>
+      <c r="BC3" s="85"/>
+      <c r="BD3" s="85"/>
+      <c r="BE3" s="85">
         <f ca="1">BE4</f>
-        <v>45453</v>
-      </c>
-      <c r="BF3" s="64"/>
-      <c r="BG3" s="64"/>
-      <c r="BH3" s="64"/>
-      <c r="BI3" s="64"/>
-      <c r="BJ3" s="64"/>
-      <c r="BK3" s="65"/>
+        <v>45488</v>
+      </c>
+      <c r="BF3" s="85"/>
+      <c r="BG3" s="85"/>
+      <c r="BH3" s="85"/>
+      <c r="BI3" s="85"/>
+      <c r="BJ3" s="85"/>
+      <c r="BK3" s="86"/>
     </row>
     <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75" t="s">
+      <c r="A4" s="73"/>
+      <c r="B4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="78" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="25">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="I4" s="25">
         <f ca="1">H4+1</f>
-        <v>45405</v>
+        <v>45440</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" ref="J4:AW4" ca="1" si="0">I4+1</f>
-        <v>45406</v>
+        <v>45441</v>
       </c>
       <c r="K4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45407</v>
+        <v>45442</v>
       </c>
       <c r="L4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45408</v>
+        <v>45443</v>
       </c>
       <c r="M4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45409</v>
+        <v>45444</v>
       </c>
       <c r="N4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45445</v>
       </c>
       <c r="O4" s="27">
         <f ca="1">N4+1</f>
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="P4" s="25">
         <f ca="1">O4+1</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="Q4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45413</v>
+        <v>45448</v>
       </c>
       <c r="R4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="S4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45415</v>
+        <v>45450</v>
       </c>
       <c r="T4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45416</v>
+        <v>45451</v>
       </c>
       <c r="U4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45417</v>
+        <v>45452</v>
       </c>
       <c r="V4" s="27">
         <f ca="1">U4+1</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="W4" s="25">
         <f ca="1">V4+1</f>
-        <v>45419</v>
+        <v>45454</v>
       </c>
       <c r="X4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45420</v>
+        <v>45455</v>
       </c>
       <c r="Y4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="Z4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45422</v>
+        <v>45457</v>
       </c>
       <c r="AA4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="AB4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="AC4" s="27">
         <f ca="1">AB4+1</f>
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="AD4" s="25">
         <f ca="1">AC4+1</f>
-        <v>45426</v>
+        <v>45461</v>
       </c>
       <c r="AE4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45427</v>
+        <v>45462</v>
       </c>
       <c r="AF4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45428</v>
+        <v>45463</v>
       </c>
       <c r="AG4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="AH4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45430</v>
+        <v>45465</v>
       </c>
       <c r="AI4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45431</v>
+        <v>45466</v>
       </c>
       <c r="AJ4" s="27">
         <f ca="1">AI4+1</f>
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="AK4" s="25">
         <f ca="1">AJ4+1</f>
-        <v>45433</v>
+        <v>45468</v>
       </c>
       <c r="AL4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="AM4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="AN4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45471</v>
       </c>
       <c r="AO4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45437</v>
+        <v>45472</v>
       </c>
       <c r="AP4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
+        <v>45473</v>
       </c>
       <c r="AQ4" s="27">
         <f ca="1">AP4+1</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="AR4" s="25">
         <f ca="1">AQ4+1</f>
-        <v>45440</v>
+        <v>45475</v>
       </c>
       <c r="AS4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45441</v>
+        <v>45476</v>
       </c>
       <c r="AT4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45442</v>
+        <v>45477</v>
       </c>
       <c r="AU4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45443</v>
+        <v>45478</v>
       </c>
       <c r="AV4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45444</v>
+        <v>45479</v>
       </c>
       <c r="AW4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45445</v>
+        <v>45480</v>
       </c>
       <c r="AX4" s="27">
         <f ca="1">AW4+1</f>
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="AY4" s="25">
         <f ca="1">AX4+1</f>
-        <v>45447</v>
+        <v>45482</v>
       </c>
       <c r="AZ4" s="25">
         <f t="shared" ref="AZ4:BD4" ca="1" si="1">AY4+1</f>
-        <v>45448</v>
+        <v>45483</v>
       </c>
       <c r="BA4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45449</v>
+        <v>45484</v>
       </c>
       <c r="BB4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45450</v>
+        <v>45485</v>
       </c>
       <c r="BC4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45451</v>
+        <v>45486</v>
       </c>
       <c r="BD4" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45452</v>
+        <v>45487</v>
       </c>
       <c r="BE4" s="27">
         <f ca="1">BD4+1</f>
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="BF4" s="25">
         <f ca="1">BE4+1</f>
-        <v>45454</v>
+        <v>45489</v>
       </c>
       <c r="BG4" s="25">
         <f t="shared" ref="BG4:BK4" ca="1" si="2">BF4+1</f>
-        <v>45455</v>
+        <v>45490</v>
       </c>
       <c r="BH4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45456</v>
+        <v>45491</v>
       </c>
       <c r="BI4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45457</v>
+        <v>45492</v>
       </c>
       <c r="BJ4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45458</v>
+        <v>45493</v>
       </c>
       <c r="BK4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45459</v>
+        <v>45494</v>
       </c>
     </row>
     <row r="5" spans="1:63" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
       <c r="H5" s="28" t="str">
         <f t="shared" ref="H5:AM5" ca="1" si="3">LEFT(TEXT(H4,"ddd"),1)</f>
         <v>M</v>
@@ -2209,7 +2214,7 @@
     </row>
     <row r="6" spans="1:63" s="35" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="69" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="31"/>
@@ -2279,7 +2284,7 @@
     </row>
     <row r="7" spans="1:63" s="35" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="64" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="36">
@@ -2287,11 +2292,11 @@
       </c>
       <c r="D7" s="50">
         <f ca="1">Project_Start</f>
-        <v>45409</v>
+        <v>45444</v>
       </c>
       <c r="E7" s="50">
         <f ca="1">D7+3</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="33">
@@ -2357,7 +2362,7 @@
     </row>
     <row r="8" spans="1:63" s="35" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="65" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="38">
@@ -2365,11 +2370,11 @@
       </c>
       <c r="D8" s="51">
         <f ca="1">E7</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="E8" s="51">
         <f ca="1">D8+2</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="33">
@@ -2435,19 +2440,19 @@
     </row>
     <row r="9" spans="1:63" s="35" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="65" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="38">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D9" s="51">
         <f ca="1">E8</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="E9" s="51">
         <f ca="1">D9+4</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="33">
@@ -2513,19 +2518,19 @@
     </row>
     <row r="10" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="65" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="51">
         <f ca="1">E9</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="E10" s="51">
         <f ca="1">D10+5</f>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="33">
@@ -2591,7 +2596,7 @@
     </row>
     <row r="11" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21"/>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="65" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="38">
@@ -2599,11 +2604,11 @@
       </c>
       <c r="D11" s="51">
         <f ca="1">D8+1</f>
-        <v>45413</v>
+        <v>45448</v>
       </c>
       <c r="E11" s="51">
         <f ca="1">D11+2</f>
-        <v>45415</v>
+        <v>45450</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33">
@@ -2669,7 +2674,7 @@
     </row>
     <row r="12" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="70" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="40"/>
@@ -2683,19 +2688,19 @@
     </row>
     <row r="13" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="66" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="42">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="53">
         <f ca="1">D11+1</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="E13" s="53">
         <f ca="1">D13+4</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="33">
@@ -2765,15 +2770,15 @@
         <v>30</v>
       </c>
       <c r="C14" s="42">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D14" s="53">
         <f ca="1">D13+2</f>
-        <v>45416</v>
+        <v>45451</v>
       </c>
       <c r="E14" s="53">
         <f ca="1">D14+5</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33">
@@ -2839,19 +2844,19 @@
     </row>
     <row r="15" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="66" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="53">
         <f ca="1">E14</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E15" s="53">
         <f ca="1">D15+3</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33">
@@ -2917,19 +2922,19 @@
     </row>
     <row r="16" spans="1:63" s="35" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="66" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="53">
         <f ca="1">D15</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E16" s="53">
         <f ca="1">D16+2</f>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33">
@@ -2995,19 +3000,19 @@
     </row>
     <row r="17" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="66" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="53">
         <f ca="1">D16</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E17" s="53">
         <f ca="1">D17+3</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33">
@@ -3073,7 +3078,7 @@
     </row>
     <row r="18" spans="1:63" s="35" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="71" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="43"/>
@@ -3143,19 +3148,19 @@
     </row>
     <row r="19" spans="1:63" s="35" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="67" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="55">
         <f ca="1">D7+15</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="E19" s="55">
         <f ca="1">D19+5</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33">
@@ -3221,19 +3226,19 @@
     </row>
     <row r="20" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="45">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D20" s="55">
         <f ca="1">E19+1</f>
-        <v>45430</v>
+        <v>45465</v>
       </c>
       <c r="E20" s="55">
         <f ca="1">D20+4</f>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33">
@@ -3299,19 +3304,19 @@
     </row>
     <row r="21" spans="1:63" s="35" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="67" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="45">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D21" s="55">
         <f ca="1">D20+5</f>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="E21" s="55">
         <f ca="1">D21+5</f>
-        <v>45440</v>
+        <v>45475</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33">
@@ -3377,7 +3382,7 @@
     </row>
     <row r="22" spans="1:63" s="35" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="72" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="46"/>
@@ -3447,19 +3452,19 @@
     </row>
     <row r="23" spans="1:63" s="35" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="68" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="48">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D23" s="57">
         <f ca="1">D19+2</f>
-        <v>45426</v>
+        <v>45461</v>
       </c>
       <c r="E23" s="57">
         <f ca="1">D23+3</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33">
@@ -3525,19 +3530,19 @@
     </row>
     <row r="24" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="68" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="48">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D24" s="57">
         <f ca="1">E23</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="E24" s="57">
         <f ca="1">D24+4</f>
-        <v>45433</v>
+        <v>45468</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33">
@@ -3603,19 +3608,19 @@
     </row>
     <row r="25" spans="1:63" s="35" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="68" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="48">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="57">
         <f ca="1">E24+1</f>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="E25" s="57">
         <f ca="1">D25+3</f>
-        <v>45437</v>
+        <v>45472</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33">
@@ -3681,7 +3686,7 @@
     </row>
     <row r="26" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="70" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="40"/>
@@ -3695,7 +3700,7 @@
     </row>
     <row r="27" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="66" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="42">
@@ -3703,11 +3708,11 @@
       </c>
       <c r="D27" s="53">
         <f ca="1">D25+1</f>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="E27" s="53">
         <f ca="1">D27+4</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="33">
@@ -3773,19 +3778,19 @@
     </row>
     <row r="28" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="66" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="42">
-        <v>0.02</v>
+        <v>0.6</v>
       </c>
       <c r="D28" s="53">
         <f ca="1">Project_Start+3</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="E28" s="53">
         <f ca="1">BA4+10</f>
-        <v>45459</v>
+        <v>45494</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
@@ -3848,19 +3853,19 @@
     </row>
     <row r="29" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="66" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="42">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D29" s="53">
         <f ca="1">E27</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="E29" s="53">
         <f ca="1">D29+18</f>
-        <v>45457</v>
+        <v>45492</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="33">
@@ -3926,11 +3931,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="P2:Y2"/>
     <mergeCell ref="P1:Y1"/>
     <mergeCell ref="H1:N1"/>
@@ -3943,6 +3943,11 @@
     <mergeCell ref="AJ3:AP3"/>
     <mergeCell ref="AQ3:AW3"/>
     <mergeCell ref="AX3:BD3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:C29">
     <cfRule type="dataBar" priority="29">
@@ -4168,23 +4173,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4500,29 +4494,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4549,9 +4543,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Added features and functionality to User Panel
</commit_message>
<xml_diff>
--- a/Project Proposal/Simple Gantt chart1.xlsx
+++ b/Project Proposal/Simple Gantt chart1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssaro\Documents\My Docs\LA Grandee BCA\4th Semester\Project\Project Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssaro\Documents\My Docs\LA Grandee BCA\4th Semester\PU-BCA-4th-Semester-Project\Project Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4813080-1451-460E-B797-3ECFAAB40C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C781DBC4-227D-4451-A8A6-140CBDAFD15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>PROGRESS</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Retrospect Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              </t>
   </si>
 </sst>
 </file>
@@ -911,15 +914,46 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="21" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -935,45 +969,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1601,387 +1604,389 @@
       <c r="D1" s="17"/>
       <c r="E1" s="18"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
       <c r="O1" s="20"/>
-      <c r="P1" s="71">
+      <c r="P1" s="82">
         <f ca="1">TODAY()-5</f>
-        <v>45409</v>
-      </c>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
+        <v>45444</v>
+      </c>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
       <c r="O2" s="20"/>
-      <c r="P2" s="69">
+      <c r="P2" s="80">
         <v>1</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
     </row>
     <row r="3" spans="1:63" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D3" s="24"/>
-      <c r="H3" s="66">
+      <c r="H3" s="87">
         <f ca="1">H4</f>
-        <v>45404</v>
-      </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64">
+        <v>45439</v>
+      </c>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85">
         <f ca="1">O4</f>
-        <v>45411</v>
-      </c>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64">
+        <v>45446</v>
+      </c>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85">
         <f ca="1">V4</f>
-        <v>45418</v>
-      </c>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64">
+        <v>45453</v>
+      </c>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85">
         <f ca="1">AC4</f>
-        <v>45425</v>
-      </c>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64">
+        <v>45460</v>
+      </c>
+      <c r="AD3" s="85"/>
+      <c r="AE3" s="85"/>
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="85"/>
+      <c r="AJ3" s="85">
         <f ca="1">AJ4</f>
-        <v>45432</v>
-      </c>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64">
+        <v>45467</v>
+      </c>
+      <c r="AK3" s="85"/>
+      <c r="AL3" s="85"/>
+      <c r="AM3" s="85"/>
+      <c r="AN3" s="85"/>
+      <c r="AO3" s="85"/>
+      <c r="AP3" s="85"/>
+      <c r="AQ3" s="85">
         <f ca="1">AQ4</f>
-        <v>45439</v>
-      </c>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="64"/>
-      <c r="AX3" s="64">
+        <v>45474</v>
+      </c>
+      <c r="AR3" s="85"/>
+      <c r="AS3" s="85"/>
+      <c r="AT3" s="85"/>
+      <c r="AU3" s="85"/>
+      <c r="AV3" s="85"/>
+      <c r="AW3" s="85"/>
+      <c r="AX3" s="85">
         <f ca="1">AX4</f>
-        <v>45446</v>
-      </c>
-      <c r="AY3" s="64"/>
-      <c r="AZ3" s="64"/>
-      <c r="BA3" s="64"/>
-      <c r="BB3" s="64"/>
-      <c r="BC3" s="64"/>
-      <c r="BD3" s="64"/>
-      <c r="BE3" s="64">
+        <v>45481</v>
+      </c>
+      <c r="AY3" s="85"/>
+      <c r="AZ3" s="85"/>
+      <c r="BA3" s="85"/>
+      <c r="BB3" s="85"/>
+      <c r="BC3" s="85"/>
+      <c r="BD3" s="85"/>
+      <c r="BE3" s="85">
         <f ca="1">BE4</f>
-        <v>45453</v>
-      </c>
-      <c r="BF3" s="64"/>
-      <c r="BG3" s="64"/>
-      <c r="BH3" s="64"/>
-      <c r="BI3" s="64"/>
-      <c r="BJ3" s="64"/>
-      <c r="BK3" s="65"/>
+        <v>45488</v>
+      </c>
+      <c r="BF3" s="85"/>
+      <c r="BG3" s="85"/>
+      <c r="BH3" s="85"/>
+      <c r="BI3" s="85"/>
+      <c r="BJ3" s="85"/>
+      <c r="BK3" s="86"/>
     </row>
     <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75" t="s">
+      <c r="A4" s="73"/>
+      <c r="B4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="78" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="25">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="I4" s="25">
         <f ca="1">H4+1</f>
-        <v>45405</v>
+        <v>45440</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" ref="J4:AW4" ca="1" si="0">I4+1</f>
-        <v>45406</v>
+        <v>45441</v>
       </c>
       <c r="K4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45407</v>
+        <v>45442</v>
       </c>
       <c r="L4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45408</v>
+        <v>45443</v>
       </c>
       <c r="M4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45409</v>
+        <v>45444</v>
       </c>
       <c r="N4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45445</v>
       </c>
       <c r="O4" s="27">
         <f ca="1">N4+1</f>
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="P4" s="25">
         <f ca="1">O4+1</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="Q4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45413</v>
+        <v>45448</v>
       </c>
       <c r="R4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="S4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45415</v>
+        <v>45450</v>
       </c>
       <c r="T4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45416</v>
+        <v>45451</v>
       </c>
       <c r="U4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45417</v>
+        <v>45452</v>
       </c>
       <c r="V4" s="27">
         <f ca="1">U4+1</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="W4" s="25">
         <f ca="1">V4+1</f>
-        <v>45419</v>
+        <v>45454</v>
       </c>
       <c r="X4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45420</v>
+        <v>45455</v>
       </c>
       <c r="Y4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="Z4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45422</v>
+        <v>45457</v>
       </c>
       <c r="AA4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="AB4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="AC4" s="27">
         <f ca="1">AB4+1</f>
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="AD4" s="25">
         <f ca="1">AC4+1</f>
-        <v>45426</v>
+        <v>45461</v>
       </c>
       <c r="AE4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45427</v>
+        <v>45462</v>
       </c>
       <c r="AF4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45428</v>
+        <v>45463</v>
       </c>
       <c r="AG4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="AH4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45430</v>
+        <v>45465</v>
       </c>
       <c r="AI4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45431</v>
+        <v>45466</v>
       </c>
       <c r="AJ4" s="27">
         <f ca="1">AI4+1</f>
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="AK4" s="25">
         <f ca="1">AJ4+1</f>
-        <v>45433</v>
+        <v>45468</v>
       </c>
       <c r="AL4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="AM4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="AN4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45471</v>
       </c>
       <c r="AO4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45437</v>
+        <v>45472</v>
       </c>
       <c r="AP4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
+        <v>45473</v>
       </c>
       <c r="AQ4" s="27">
         <f ca="1">AP4+1</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="AR4" s="25">
         <f ca="1">AQ4+1</f>
-        <v>45440</v>
+        <v>45475</v>
       </c>
       <c r="AS4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45441</v>
+        <v>45476</v>
       </c>
       <c r="AT4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45442</v>
+        <v>45477</v>
       </c>
       <c r="AU4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45443</v>
+        <v>45478</v>
       </c>
       <c r="AV4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>45444</v>
+        <v>45479</v>
       </c>
       <c r="AW4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45445</v>
+        <v>45480</v>
       </c>
       <c r="AX4" s="27">
         <f ca="1">AW4+1</f>
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="AY4" s="25">
         <f ca="1">AX4+1</f>
-        <v>45447</v>
+        <v>45482</v>
       </c>
       <c r="AZ4" s="25">
         <f t="shared" ref="AZ4:BD4" ca="1" si="1">AY4+1</f>
-        <v>45448</v>
+        <v>45483</v>
       </c>
       <c r="BA4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45449</v>
+        <v>45484</v>
       </c>
       <c r="BB4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45450</v>
+        <v>45485</v>
       </c>
       <c r="BC4" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>45451</v>
+        <v>45486</v>
       </c>
       <c r="BD4" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45452</v>
+        <v>45487</v>
       </c>
       <c r="BE4" s="27">
         <f ca="1">BD4+1</f>
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="BF4" s="25">
         <f ca="1">BE4+1</f>
-        <v>45454</v>
+        <v>45489</v>
       </c>
       <c r="BG4" s="25">
         <f t="shared" ref="BG4:BK4" ca="1" si="2">BF4+1</f>
-        <v>45455</v>
+        <v>45490</v>
       </c>
       <c r="BH4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45456</v>
+        <v>45491</v>
       </c>
       <c r="BI4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45457</v>
+        <v>45492</v>
       </c>
       <c r="BJ4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45458</v>
+        <v>45493</v>
       </c>
       <c r="BK4" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>45459</v>
+        <v>45494</v>
       </c>
     </row>
     <row r="5" spans="1:63" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
       <c r="H5" s="28" t="str">
         <f t="shared" ref="H5:AM5" ca="1" si="3">LEFT(TEXT(H4,"ddd"),1)</f>
         <v>M</v>
@@ -2209,7 +2214,7 @@
     </row>
     <row r="6" spans="1:63" s="35" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="69" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="31"/>
@@ -2279,7 +2284,7 @@
     </row>
     <row r="7" spans="1:63" s="35" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="64" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="36">
@@ -2287,11 +2292,11 @@
       </c>
       <c r="D7" s="50">
         <f ca="1">Project_Start</f>
-        <v>45409</v>
+        <v>45444</v>
       </c>
       <c r="E7" s="50">
         <f ca="1">D7+3</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="33">
@@ -2357,7 +2362,7 @@
     </row>
     <row r="8" spans="1:63" s="35" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="65" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="38">
@@ -2365,11 +2370,11 @@
       </c>
       <c r="D8" s="51">
         <f ca="1">E7</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="E8" s="51">
         <f ca="1">D8+2</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="33">
@@ -2435,19 +2440,19 @@
     </row>
     <row r="9" spans="1:63" s="35" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="65" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="38">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D9" s="51">
         <f ca="1">E8</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="E9" s="51">
         <f ca="1">D9+4</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="33">
@@ -2513,19 +2518,19 @@
     </row>
     <row r="10" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="65" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="51">
         <f ca="1">E9</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="E10" s="51">
         <f ca="1">D10+5</f>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="33">
@@ -2591,7 +2596,7 @@
     </row>
     <row r="11" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21"/>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="65" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="38">
@@ -2599,11 +2604,11 @@
       </c>
       <c r="D11" s="51">
         <f ca="1">D8+1</f>
-        <v>45413</v>
+        <v>45448</v>
       </c>
       <c r="E11" s="51">
         <f ca="1">D11+2</f>
-        <v>45415</v>
+        <v>45450</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33">
@@ -2669,7 +2674,7 @@
     </row>
     <row r="12" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="70" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="40"/>
@@ -2683,19 +2688,19 @@
     </row>
     <row r="13" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="66" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="42">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="53">
         <f ca="1">D11+1</f>
-        <v>45414</v>
+        <v>45449</v>
       </c>
       <c r="E13" s="53">
         <f ca="1">D13+4</f>
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="33">
@@ -2765,15 +2770,15 @@
         <v>30</v>
       </c>
       <c r="C14" s="42">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D14" s="53">
         <f ca="1">D13+2</f>
-        <v>45416</v>
+        <v>45451</v>
       </c>
       <c r="E14" s="53">
         <f ca="1">D14+5</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33">
@@ -2839,19 +2844,19 @@
     </row>
     <row r="15" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="66" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="53">
         <f ca="1">E14</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E15" s="53">
         <f ca="1">D15+3</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33">
@@ -2917,19 +2922,19 @@
     </row>
     <row r="16" spans="1:63" s="35" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="66" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="53">
         <f ca="1">D15</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E16" s="53">
         <f ca="1">D16+2</f>
-        <v>45423</v>
+        <v>45458</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33">
@@ -2995,19 +3000,19 @@
     </row>
     <row r="17" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="66" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="53">
         <f ca="1">D16</f>
-        <v>45421</v>
+        <v>45456</v>
       </c>
       <c r="E17" s="53">
         <f ca="1">D17+3</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33">
@@ -3073,7 +3078,7 @@
     </row>
     <row r="18" spans="1:63" s="35" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="71" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="43"/>
@@ -3143,19 +3148,19 @@
     </row>
     <row r="19" spans="1:63" s="35" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="67" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="55">
         <f ca="1">D7+15</f>
-        <v>45424</v>
+        <v>45459</v>
       </c>
       <c r="E19" s="55">
         <f ca="1">D19+5</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33">
@@ -3221,19 +3226,19 @@
     </row>
     <row r="20" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="45">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D20" s="55">
         <f ca="1">E19+1</f>
-        <v>45430</v>
+        <v>45465</v>
       </c>
       <c r="E20" s="55">
         <f ca="1">D20+4</f>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33">
@@ -3299,19 +3304,19 @@
     </row>
     <row r="21" spans="1:63" s="35" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="67" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="45">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D21" s="55">
         <f ca="1">D20+5</f>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="E21" s="55">
         <f ca="1">D21+5</f>
-        <v>45440</v>
+        <v>45475</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33">
@@ -3377,7 +3382,7 @@
     </row>
     <row r="22" spans="1:63" s="35" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="72" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="46"/>
@@ -3447,19 +3452,19 @@
     </row>
     <row r="23" spans="1:63" s="35" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="68" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="48">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D23" s="57">
         <f ca="1">D19+2</f>
-        <v>45426</v>
+        <v>45461</v>
       </c>
       <c r="E23" s="57">
         <f ca="1">D23+3</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33">
@@ -3525,19 +3530,19 @@
     </row>
     <row r="24" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="68" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="48">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D24" s="57">
         <f ca="1">E23</f>
-        <v>45429</v>
+        <v>45464</v>
       </c>
       <c r="E24" s="57">
         <f ca="1">D24+4</f>
-        <v>45433</v>
+        <v>45468</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33">
@@ -3603,19 +3608,19 @@
     </row>
     <row r="25" spans="1:63" s="35" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="68" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="48">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="57">
         <f ca="1">E24+1</f>
-        <v>45434</v>
+        <v>45469</v>
       </c>
       <c r="E25" s="57">
         <f ca="1">D25+3</f>
-        <v>45437</v>
+        <v>45472</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33">
@@ -3681,7 +3686,7 @@
     </row>
     <row r="26" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="70" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="40"/>
@@ -3695,7 +3700,7 @@
     </row>
     <row r="27" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="66" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="42">
@@ -3703,11 +3708,11 @@
       </c>
       <c r="D27" s="53">
         <f ca="1">D25+1</f>
-        <v>45435</v>
+        <v>45470</v>
       </c>
       <c r="E27" s="53">
         <f ca="1">D27+4</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="33">
@@ -3773,19 +3778,19 @@
     </row>
     <row r="28" spans="1:63" s="35" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="66" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="42">
-        <v>0.02</v>
+        <v>0.6</v>
       </c>
       <c r="D28" s="53">
         <f ca="1">Project_Start+3</f>
-        <v>45412</v>
+        <v>45447</v>
       </c>
       <c r="E28" s="53">
         <f ca="1">BA4+10</f>
-        <v>45459</v>
+        <v>45494</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
@@ -3848,19 +3853,19 @@
     </row>
     <row r="29" spans="1:63" s="35" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="66" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="42">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D29" s="53">
         <f ca="1">E27</f>
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="E29" s="53">
         <f ca="1">D29+18</f>
-        <v>45457</v>
+        <v>45492</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="33">
@@ -3926,11 +3931,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="P2:Y2"/>
     <mergeCell ref="P1:Y1"/>
     <mergeCell ref="H1:N1"/>
@@ -3943,6 +3943,11 @@
     <mergeCell ref="AJ3:AP3"/>
     <mergeCell ref="AQ3:AW3"/>
     <mergeCell ref="AX3:BD3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:C29">
     <cfRule type="dataBar" priority="29">
@@ -4168,23 +4173,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4500,29 +4494,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4549,9 +4543,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>